<commit_message>
updated parts list and contents
</commit_message>
<xml_diff>
--- a/instructional documents/Cercospora Bill of Material.xlsx
+++ b/instructional documents/Cercospora Bill of Material.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://colostate.sharepoint.com/sites/AWQP_Sharepoint/Shared Documents/Water_Quality_Project/Research/PileTemp_Cercospora Systems/Sensor Build Info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansleybr\Documents\GitHub\awqp-loggers\instructional documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="8_{EBAD83C9-180D-44F8-8826-BC14838E2C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAFBDF71-1E19-4D14-AFF8-A7547FA0499C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7579689-45A1-4C66-8FE6-46C04C7A654A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{80D2ED8C-A0A6-4A18-8669-4CE8FFF698BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" firstSheet="1" activeTab="1" xr2:uid="{80D2ED8C-A0A6-4A18-8669-4CE8FFF698BE}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="84">
   <si>
     <t>Main Items</t>
   </si>
@@ -225,15 +225,6 @@
     <t>https://www.homedepot.com/p/Halex-Universal-3-4-in-1-Hole-Strap-4-Pack-22107/314968705?source=shoppingads&amp;locale=en-US&amp;pla&amp;mtc=SHOPPING-BF-CDP-GGL-D27-027_006_CONDUIT_FIT-NA-NA-NA-PMAX-NA-NA-NA-NA-NBR-NA-NA-NEW-NA_D27Transition&amp;cm_mmc=SHOPPING-BF-CDP-GGL-D27-027_006_CONDUIT_FIT-NA-NA-NA-PMAX-NA-NA-NA-NA-NBR-NA-NA-NEW-NA_D27Transition-71700000113157690--&amp;gad_source=1&amp;acs_info=ZmluYWxfdXJsOiAiaHR0cHM6Ly93d3cuaG9tZWRlcG90LmNvbS9wL0hhbGV4LVVuaXZlcnNhbC0zLTQtaW4tMS1Ib2xlLVN0cmFwLTQtUGFjay0yMjEwNy8zMTQ5Njg3MDUiCg&amp;gclid=Cj0KCQiAh8OtBhCQARIsAIkWb6-ZNUGk4DF6_8K9b_SG3twg-_4rTYJGDSozB688e1TayXbsJCpro0IaAm47EALw_wcB&amp;gclsrc=aw.ds</t>
   </si>
   <si>
-    <t>Cone Drill bit or 1/2" drill bit</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/CO-Z-Titanium-Drilling-Cutting-Electrician/dp/B076QC5BWR/ref=sxin_14_pa_sp_search_thematic_sspa?content-id=amzn1.sym.92181fe7-c843-4c1b-b489-84c087a93895%3Aamzn1.sym.92181fe7-c843-4c1b-b489-84c087a93895&amp;crid=2U01GZIGM67DL&amp;cv_ct_cx=cone+drill+bit&amp;keywords=cone+drill+bit&amp;pd_rd_i=B076QC5BWR&amp;pd_rd_r=557b2ca0-8959-460e-91cf-71f9f81a8c58&amp;pd_rd_w=N3oPN&amp;pd_rd_wg=O6cNx&amp;pf_rd_p=92181fe7-c843-4c1b-b489-84c087a93895&amp;pf_rd_r=WGYSVA5CQWX46TTP7JY3&amp;qid=1706724546&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sprefix=cone+dril%2Caps%2C165&amp;sr=1-5-364cf978-ce2a-480a-9bb0-bdb96faa0f61-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9zZWFyY2hfdGhlbWF0aWM&amp;psc=1</t>
-  </si>
-  <si>
-    <t>Heat gun or lighter</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -250,6 +241,54 @@
   </si>
   <si>
     <t>E.Deleon@colostate.edu</t>
+  </si>
+  <si>
+    <t>Recommended Tools</t>
+  </si>
+  <si>
+    <t>Cone Drill Bit</t>
+  </si>
+  <si>
+    <t>https://a.co/d/d9EyOLx</t>
+  </si>
+  <si>
+    <t>Magnetic Soldering Alligator Clips</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/KOTTO-Soldering-Magnetic-Flexible-Workshop/dp/B083SFWLW7/ref=sr_1_97?crid=1W1WI7KFN5MOK&amp;keywords=magnetic%2Balligator%2Bclips&amp;qid=1707339995&amp;sprefix=magnetic%2Balli%2Caps%2C106&amp;sr=8-97&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/IRWIN-VISE-GRIP-2078300-Self-Adjusting-Stripper/dp/B000OQ21CA/ref=sr_1_15?crid=379UHPQLB7G9D&amp;keywords=wire%2Bstripper&amp;qid=1707340653&amp;sprefix=wire%2Bs%2Caps%2C123&amp;sr=8-15&amp;th=1</t>
+  </si>
+  <si>
+    <t>Wire Stripper</t>
+  </si>
+  <si>
+    <t>Mini Heat Gun</t>
+  </si>
+  <si>
+    <t>Magnifying Glass w/ Light</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/SEEKONE-Handheld-Reflector-Embossing-Stripping/dp/B08VFY8THD/ref=sr_1_5?crid=3R62NG61UYLY0&amp;keywords=mini+heat+gun&amp;qid=1707340837&amp;sprefix=mini+heat+gun%2Caps%2C94&amp;sr=8-5</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Magnifying-Reading-Dimmable-Eye-Caring-Headboard/dp/B09M9YYSGB/ref=sr_1_42?crid=39IAFATUH0IKY&amp;keywords=magnifying%2Bglass%2Bwith%2Blight&amp;qid=1707342855&amp;sprefix=magni%2Caps%2C112&amp;sr=8-42&amp;th=1</t>
+  </si>
+  <si>
+    <t>#6 x ½” Sheet Metal Screws</t>
+  </si>
+  <si>
+    <t>100 pk</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Stainless-Phillips-Tapping-Bright-Finish/dp/B08LV1M9FC/ref=sr_1_3?crid=LCO1S41XKHLI&amp;keywords=%236%2B1%2F2%2Bin%2Bsheet%2Bmetal%2Bscrews&amp;qid=1707341265&amp;sprefix=%2B6%2B1%2F2%2Bin%2Bsheet%2Bmetal%2Bscrews%2Caps%2C112&amp;sr=8-3&amp;th=1</t>
+  </si>
+  <si>
+    <t>Radiation Shield (Amazon Version)</t>
+  </si>
+  <si>
+    <t>https://a.co/d/9YjHxkh</t>
   </si>
 </sst>
 </file>
@@ -260,7 +299,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,7 +339,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -326,13 +365,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -375,6 +423,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -699,7 +759,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" style="2" customWidth="1"/>
@@ -708,15 +768,15 @@
     <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -730,7 +790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -744,7 +804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -758,7 +818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -772,7 +832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -786,7 +846,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -800,7 +860,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -814,7 +874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -825,7 +885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -839,7 +899,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -853,7 +913,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -867,7 +927,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -881,15 +941,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="15" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -903,7 +963,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -917,7 +977,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -931,7 +991,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -945,7 +1005,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -959,7 +1019,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -973,7 +1033,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -987,7 +1047,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -1012,13 +1072,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D96A2117-29E3-4FE2-AB8A-EAB84811DFDE}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="8.85546875" style="5"/>
@@ -1028,23 +1088,23 @@
     <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="1:7" ht="15">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1067,7 +1127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1092,7 +1152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1103,21 +1163,21 @@
         <v>47</v>
       </c>
       <c r="D5" s="5">
-        <f t="shared" ref="D5:D10" si="0">B5</f>
+        <f t="shared" ref="D5:D11" si="0">B5</f>
         <v>2.5</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" ref="F5:F10" si="1">D5*E5</f>
+        <f t="shared" ref="F5:F11" si="1">D5*E5</f>
         <v>2.5</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1142,7 +1202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1167,7 +1227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1192,7 +1252,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1217,7 +1277,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1242,327 +1302,424 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15">
-      <c r="A12" s="15" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="5">
+        <v>22.1</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>22.1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="1"/>
+        <v>22.1</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-    </row>
-    <row r="13" spans="1:7" ht="15">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="6">
+        <v>7.99</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="5">
+        <f>B14/100</f>
+        <v>7.9899999999999999E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6">
+        <f>D14*E14</f>
+        <v>7.9899999999999999E-2</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B15" s="5">
         <v>9.99</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="5">
-        <f>B13/30</f>
+      <c r="D15" s="5">
+        <f>B15/30</f>
         <v>0.33300000000000002</v>
       </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6">
-        <f>D13*E13</f>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6">
+        <f>D15*E15</f>
         <v>0.33300000000000002</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15">
-      <c r="A14" s="1" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B16" s="5">
         <v>33.99</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="5">
-        <f>B14/500</f>
+      <c r="D16" s="5">
+        <f>B16/500</f>
         <v>6.7979999999999999E-2</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E16" s="1">
         <v>4</v>
       </c>
-      <c r="F14" s="6">
-        <f t="shared" ref="F14:F21" si="2">D14*E14</f>
+      <c r="F16" s="6">
+        <f t="shared" ref="F16:F21" si="2">D16*E16</f>
         <v>0.27192</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15">
-      <c r="A15" s="1" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B17" s="5">
         <v>21.55</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="5">
-        <f>B15/50</f>
+      <c r="D17" s="5">
+        <f>B17/50</f>
         <v>0.43099999999999999</v>
       </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6">
         <f t="shared" si="2"/>
         <v>0.43099999999999999</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15">
-      <c r="A16" s="1" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B18" s="5">
         <v>27.88</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="5">
-        <f>B16/65</f>
+      <c r="D18" s="5">
+        <f>B18/65</f>
         <v>0.42892307692307691</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E18" s="1">
         <v>7</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F18" s="6">
         <f t="shared" si="2"/>
         <v>3.0024615384615383</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15">
-      <c r="A17" s="1" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B19" s="5">
         <v>7.99</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="5">
-        <f>B17/20</f>
+      <c r="D19" s="5">
+        <f>B19/20</f>
         <v>0.39950000000000002</v>
       </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6">
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6">
         <f t="shared" si="2"/>
         <v>0.39950000000000002</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15">
-      <c r="A18" s="1" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B20" s="5">
         <v>8.59</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="5">
-        <f>B18/5</f>
+      <c r="D20" s="5">
+        <f>B20/5</f>
         <v>1.718</v>
       </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="6">
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6">
         <f t="shared" si="2"/>
         <v>1.718</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15">
-      <c r="A19" s="1" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B21" s="5">
         <v>5.99</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="5">
-        <f>B19/60</f>
+      <c r="D21" s="5">
+        <f>B21/60</f>
         <v>9.9833333333333343E-2</v>
       </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19" s="6">
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6">
         <f t="shared" si="2"/>
         <v>9.9833333333333343E-2</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15">
-      <c r="A20" s="1" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B22" s="5">
         <v>2.5</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="5">
-        <f>B20/4</f>
+      <c r="D22" s="5">
+        <f>B22/4</f>
         <v>0.625</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E22" s="1">
         <v>2</v>
       </c>
-      <c r="F20" s="6">
-        <f>D20*E20</f>
+      <c r="F22" s="6">
+        <f>D22*E22</f>
         <v>1.25</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15">
-      <c r="A21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="5">
-        <v>9.99</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="5">
-        <f>B21</f>
-        <v>9.99</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="6">
-        <f t="shared" si="2"/>
-        <v>9.99</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15">
-      <c r="A22" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="7" customFormat="1">
+    <row r="23" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" ht="15">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B24" s="12">
-        <f>SUM(B13:B21,B4:B10)</f>
-        <v>266.79999999999995</v>
+        <f>SUM(B14:B22,B4:B11)</f>
+        <v>286.89999999999998</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="12"/>
       <c r="E24" s="11"/>
       <c r="F24" s="12">
-        <f>SUM(F13:F21,F4:F10)</f>
-        <v>175.77571487179489</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <f>SUM(F14:F22,F4:F11)</f>
+        <v>187.96561487179488</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="5">
+        <v>10.99</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="5">
+        <v>21.99</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="5">
+        <v>25.99</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="5">
+        <v>24.99</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="5">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="16">
+        <f>SUM(B28:B32)</f>
+        <v>103.94999999999999</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="3" t="s">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15">
-      <c r="A29" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15">
-      <c r="A30" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A27:G27"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G19" r:id="rId1" xr:uid="{50608113-C209-4C4A-87F2-FEA94D41E8CE}"/>
-    <hyperlink ref="A29" r:id="rId2" xr:uid="{CF27A860-8EB6-4609-9AAF-08650E20187A}"/>
-    <hyperlink ref="A30" r:id="rId3" xr:uid="{55FE673A-BC99-49AB-A11C-E8202D9DBC9E}"/>
+    <hyperlink ref="G21" r:id="rId1" xr:uid="{50608113-C209-4C4A-87F2-FEA94D41E8CE}"/>
+    <hyperlink ref="A38" r:id="rId2" xr:uid="{CF27A860-8EB6-4609-9AAF-08650E20187A}"/>
+    <hyperlink ref="A39" r:id="rId3" xr:uid="{55FE673A-BC99-49AB-A11C-E8202D9DBC9E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="167cb1e9-24b5-43e0-9f5d-14a54474cc90">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fbf6f0f6-9634-473c-8838-2f74fc79f714" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100678F2DA36292A241BB6B602A04ACAAD9" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e65193b06eae86f79c3903a4a9f0dcf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="167cb1e9-24b5-43e0-9f5d-14a54474cc90" xmlns:ns3="fbf6f0f6-9634-473c-8838-2f74fc79f714" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03593a2a675d04ffa4dc626c9c15704c" ns2:_="" ns3:_="">
     <xsd:import namespace="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
@@ -1817,14 +1974,60 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="167cb1e9-24b5-43e0-9f5d-14a54474cc90">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fbf6f0f6-9634-473c-8838-2f74fc79f714" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BD73F7C-F428-40BF-8E52-A9BC4D2C983C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1E81F03-6419-4048-A634-C688504EC386}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
+    <ds:schemaRef ds:uri="fbf6f0f6-9634-473c-8838-2f74fc79f714"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6FE033F-E9EE-49D3-A665-ABA46FC899E9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6FE033F-E9EE-49D3-A665-ABA46FC899E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
+    <ds:schemaRef ds:uri="fbf6f0f6-9634-473c-8838-2f74fc79f714"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1E81F03-6419-4048-A634-C688504EC386}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BD73F7C-F428-40BF-8E52-A9BC4D2C983C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>